<commit_message>
Nachbearbeitung und NRMSD Vergleich
</commit_message>
<xml_diff>
--- a/Durchläufe/Neue Gewichtung/Ohne Fehler/Vergleich alt  vs neue gewichtung.xlsx
+++ b/Durchläufe/Neue Gewichtung/Ohne Fehler/Vergleich alt  vs neue gewichtung.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim Schell\Documents\GitHub\Limits-to-Growth-Masterprojekt-TH-Koeln-2022\Durchläufe\Neue Gewichtung\Ohne Fehler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72E1D65A-D316-4B2A-96F9-7BEDD8865AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CED116E3-EED2-4039-94D3-C9D06A84746D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="4" r:id="rId1"/>
+    <sheet name="Gewichtung" sheetId="4" r:id="rId1"/>
     <sheet name="NRI Default" sheetId="1" r:id="rId2"/>
     <sheet name="NRI mal 2" sheetId="2" r:id="rId3"/>
     <sheet name="Komplett" sheetId="3" r:id="rId4"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="63">
   <si>
     <t>alt</t>
   </si>
@@ -228,16 +228,13 @@
   </si>
   <si>
     <t>Ecological_Footprint</t>
-  </si>
-  <si>
-    <t>x</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +262,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -319,13 +322,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -333,6 +333,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2051,7 +2055,7 @@
                   <c:v>0.33179999999999998</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>0.34739999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3950,16 +3954,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>4762</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>757237</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>1704975</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>1695450</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4253,7 +4257,7 @@
   <dimension ref="A2:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4262,10 +4266,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="3"/>
+      <c r="C2" s="6"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -4276,7 +4280,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>48</v>
       </c>
       <c r="B4">
@@ -4285,11 +4289,11 @@
       <c r="C4">
         <v>1</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>49</v>
       </c>
       <c r="B5">
@@ -4298,11 +4302,11 @@
       <c r="C5">
         <v>0</v>
       </c>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>50</v>
       </c>
       <c r="B6">
@@ -4311,11 +4315,11 @@
       <c r="C6">
         <v>0.75</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>51</v>
       </c>
       <c r="B7">
@@ -4324,11 +4328,11 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B8">
@@ -4337,11 +4341,11 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>53</v>
       </c>
       <c r="B9">
@@ -4350,11 +4354,11 @@
       <c r="C9">
         <v>0.5</v>
       </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>54</v>
       </c>
       <c r="B10">
@@ -4363,11 +4367,11 @@
       <c r="C10">
         <v>0</v>
       </c>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>55</v>
       </c>
       <c r="B11">
@@ -4376,11 +4380,11 @@
       <c r="C11">
         <v>0.5</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>56</v>
       </c>
       <c r="B12">
@@ -4389,11 +4393,11 @@
       <c r="C12">
         <v>0</v>
       </c>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>57</v>
       </c>
       <c r="B13">
@@ -4402,11 +4406,11 @@
       <c r="C13">
         <v>0.5</v>
       </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>58</v>
       </c>
       <c r="B14">
@@ -4415,11 +4419,11 @@
       <c r="C14">
         <v>0</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B15">
@@ -4428,11 +4432,11 @@
       <c r="C15">
         <v>0.5</v>
       </c>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B16">
@@ -4441,11 +4445,11 @@
       <c r="C16">
         <v>0</v>
       </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="A17" s="5" t="s">
         <v>61</v>
       </c>
       <c r="B17">
@@ -4454,11 +4458,11 @@
       <c r="C17">
         <v>0.75</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>62</v>
       </c>
       <c r="B18">
@@ -4467,8 +4471,8 @@
       <c r="C18">
         <v>0.75</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4482,8 +4486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:F38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4494,10 +4498,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
@@ -5133,7 +5137,7 @@
   <dimension ref="B1:F38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D3"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5143,10 +5147,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
@@ -5782,7 +5786,7 @@
   <dimension ref="C3:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5794,10 +5798,10 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
     </row>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
@@ -5835,8 +5839,8 @@
       <c r="G5" s="2">
         <v>0.33179999999999998</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>63</v>
+      <c r="H5" s="7">
+        <v>0.34739999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>